<commit_message>
fix get all data excel change to get last once
</commit_message>
<xml_diff>
--- a/bin/Debug/data.xlsx
+++ b/bin/Debug/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\Workshop\Visual Studio\Final Project\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D919F16-E9EF-4B85-BAF1-EFDB361E97D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED6A7F1-8A29-4FB5-86A0-14423BF118DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,25 +47,25 @@
   <si>
     <t xml:space="preserve">คุณสั่งชื้อ MacBook Air 
 โดยมี 
+Chip: Macbook Air M2 
+Color: Silver 
+ในราคา: 55000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">คุณสั่งชื้อ MacBook Air 
+โดยมี 
 Chip: Macbook Air M1 
-Color: Starlight 
+Color: Midnight 
 ในราคา: 55000</t>
   </si>
   <si>
     <t xml:space="preserve">คุณสั่งชื้อ Asus Tuf Gaming F15 
 โดยมี 
-cpu: Intel core I5 gen 10 
-ram: 16GB 
+cpu: Intel core I5 gen 9 
+ram: 8GB 
 disk: 512GB SSD 
 gpu:NVIDIA GeForce GTX 1650 
 ในราคา: 35000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">คุณสั่งชื้อ MacBook Air 
-โดยมี 
-Chip: Macbook Air M2 
-Color: Midnight 
-ในราคา: 55000</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,12 +412,12 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">

</xml_diff>